<commit_message>
accommodating changed input data
</commit_message>
<xml_diff>
--- a/data/input/DOC_20220226_AT46_wData20220307.xlsx
+++ b/data/input/DOC_20220226_AT46_wData20220307.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sosiknas1\Lab_data\LTER\DOC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E9A79B-E110-46FE-A904-8EDFAD531025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4108801F-F51A-41D6-9E85-BF2DE32E9D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
   <si>
     <t>AT46</t>
   </si>
@@ -33,9 +33,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>L4</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>LTER Station</t>
   </si>
   <si>
-    <t>Cast Type</t>
-  </si>
-  <si>
     <t>Cast</t>
   </si>
   <si>
@@ -250,6 +244,15 @@
   </si>
   <si>
     <t>BLANK; Atlantis Hydro Lab milliQ; acidified 60uL; same acid vial used throughout cruise</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>quality_flag</t>
   </si>
 </sst>
 </file>
@@ -348,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +385,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,71 +668,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="L2" sqref="L2:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" customWidth="1"/>
-    <col min="12" max="12" width="3" style="11" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="59.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="3" style="11" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -755,25 +765,28 @@
         <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="8">
+        <v>66</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="8">
         <v>44623</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="10">
+      <c r="O2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="10">
         <v>90.7838052588273</v>
       </c>
-      <c r="P2" s="10">
+      <c r="Q2" s="10">
         <v>6.1191052274216</v>
       </c>
-      <c r="Q2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -802,25 +815,28 @@
         <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" s="8">
+        <v>66</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="8">
         <v>44623</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="10">
         <v>85.851976872899101</v>
       </c>
-      <c r="P3" s="10">
+      <c r="Q3" s="10">
         <v>5.0875635505130399</v>
       </c>
-      <c r="Q3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,10 +850,10 @@
         <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
@@ -849,22 +865,25 @@
         <v>59</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="8">
+        <v>66</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="8">
         <v>44623</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="10">
         <v>80.993538790332906</v>
       </c>
-      <c r="P4" s="10">
+      <c r="Q4" s="10">
         <v>7.3858384066653198</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,10 +897,10 @@
         <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -893,22 +912,25 @@
         <v>38</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" s="8">
+        <v>66</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
         <v>44624</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" s="10">
         <v>82.449704082883585</v>
       </c>
-      <c r="P5" s="10">
+      <c r="Q5" s="10">
         <v>8.3443321729389623</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,10 +944,10 @@
         <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -937,25 +959,28 @@
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="8">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="8">
         <v>44624</v>
       </c>
-      <c r="N6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="10">
         <v>81.14914060931946</v>
       </c>
-      <c r="P6" s="10">
+      <c r="Q6" s="10">
         <v>7.6653512721553119</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,10 +994,10 @@
         <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
@@ -984,22 +1009,25 @@
         <v>52</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7" s="8">
+        <v>66</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8">
         <v>44624</v>
       </c>
-      <c r="N7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="10">
         <v>76.033590946634263</v>
       </c>
-      <c r="P7" s="10">
+      <c r="Q7" s="10">
         <v>9.1280940769299725</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,10 +1041,10 @@
         <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G8" s="1">
         <v>3</v>
@@ -1028,22 +1056,25 @@
         <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" s="8">
+        <v>66</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8">
         <v>44623</v>
       </c>
-      <c r="N8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="10">
         <v>74.637938519181404</v>
       </c>
-      <c r="P8" s="10">
+      <c r="Q8" s="10">
         <v>8.8712584214136498</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1057,10 +1088,10 @@
         <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G9" s="1">
         <v>6</v>
@@ -1072,22 +1103,25 @@
         <v>22</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="8">
+        <v>66</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="8">
         <v>44623</v>
       </c>
-      <c r="N9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="10">
         <v>74.006781910268003</v>
       </c>
-      <c r="P9" s="10">
+      <c r="Q9" s="10">
         <v>8.1285484140394804</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1101,10 +1135,10 @@
         <v>94</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G10" s="1">
         <v>6</v>
@@ -1116,22 +1150,25 @@
         <v>2</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M10" s="8">
+        <v>66</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="8">
         <v>44623</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="10">
         <v>70.850998865700802</v>
       </c>
-      <c r="P10" s="10">
+      <c r="Q10" s="10">
         <v>8.7639780870151593</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,10 +1182,10 @@
         <v>1590</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G11" s="1">
         <v>7</v>
@@ -1160,22 +1197,25 @@
         <v>500</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M11" s="8">
+        <v>66</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8">
         <v>44623</v>
       </c>
-      <c r="N11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="10">
         <v>49.949440468195498</v>
       </c>
-      <c r="P11" s="10">
+      <c r="Q11" s="10">
         <v>23.4696362330236</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1189,10 +1229,10 @@
         <v>1590</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G12" s="1">
         <v>7</v>
@@ -1204,25 +1244,28 @@
         <v>500</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="8">
+        <v>19</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8">
         <v>44624</v>
       </c>
-      <c r="N12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="10">
         <v>48.360490370244072</v>
       </c>
-      <c r="P12" s="10">
+      <c r="Q12" s="10">
         <v>24.266853420328431</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,10 +1279,10 @@
         <v>1590</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G13" s="1">
         <v>7</v>
@@ -1251,22 +1294,25 @@
         <v>100</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="8">
+        <v>66</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="8">
         <v>44623</v>
       </c>
-      <c r="N13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="10">
         <v>73.889357424888701</v>
       </c>
-      <c r="P13" s="10">
+      <c r="Q13" s="10">
         <v>11.338706112578899</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1280,10 +1326,10 @@
         <v>1590</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G14" s="1">
         <v>7</v>
@@ -1295,22 +1341,25 @@
         <v>45</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="8">
+        <v>66</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="8">
         <v>44624</v>
       </c>
-      <c r="N14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="10">
         <v>64.718688726627164</v>
       </c>
-      <c r="P14" s="10">
+      <c r="Q14" s="10">
         <v>10.838120049273932</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,10 +1373,10 @@
         <v>1590</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G15" s="1">
         <v>7</v>
@@ -1339,22 +1388,25 @@
         <v>2</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M15" s="8">
+        <v>66</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="8">
         <v>44623</v>
       </c>
-      <c r="N15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="10">
         <v>69.882246861322102</v>
       </c>
-      <c r="P15" s="10">
+      <c r="Q15" s="10">
         <v>11.6522947823591</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1368,10 +1420,10 @@
         <v>140</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G16" s="1">
         <v>8</v>
@@ -1383,25 +1435,28 @@
         <v>28</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="8">
+        <v>23</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16" s="8">
         <v>44624</v>
       </c>
-      <c r="N16" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="P16" s="10">
         <v>71.95849206280036</v>
       </c>
-      <c r="P16" s="10">
+      <c r="Q16" s="10">
         <v>9.1825801985977922</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1415,10 +1470,10 @@
         <v>140</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1">
         <v>8</v>
@@ -1430,25 +1485,28 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="8">
+        <v>23</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="N17" s="8">
         <v>44624</v>
       </c>
-      <c r="N17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="O17" s="10">
+      <c r="O17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" s="10">
         <v>75.108745809877661</v>
       </c>
-      <c r="P17" s="10">
+      <c r="Q17" s="10">
         <v>8.5580854194819622</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1462,10 +1520,10 @@
         <v>412</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G18" s="1">
         <v>9</v>
@@ -1477,22 +1535,25 @@
         <v>37</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M18" s="8">
+        <v>66</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="8">
         <v>44624</v>
       </c>
-      <c r="N18" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="O18" s="10">
+      <c r="O18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P18" s="10">
         <v>71.192604683923776</v>
       </c>
-      <c r="P18" s="10">
+      <c r="Q18" s="10">
         <v>8.6712489029459121</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,10 +1567,10 @@
         <v>412</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G19" s="1">
         <v>9</v>
@@ -1521,22 +1582,25 @@
         <v>25</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M19" s="8">
+        <v>66</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" s="8">
         <v>44624</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="O19" s="10">
+      <c r="O19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P19" s="10">
         <v>71.20705538918557</v>
       </c>
-      <c r="P19" s="10">
+      <c r="Q19" s="10">
         <v>8.0090329626754304</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1550,10 +1614,10 @@
         <v>412</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G20" s="1">
         <v>9</v>
@@ -1565,22 +1629,25 @@
         <v>2</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M20" s="8">
+        <v>66</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="8">
         <v>44624</v>
       </c>
-      <c r="N20" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P20" s="10">
         <v>69.574125694599559</v>
       </c>
-      <c r="P20" s="10">
+      <c r="Q20" s="10">
         <v>8.331758452554082</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1594,10 +1661,10 @@
         <v>135</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G21" s="1">
         <v>13</v>
@@ -1609,22 +1676,25 @@
         <v>57</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M21" s="8">
+        <v>66</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="N21" s="8">
         <v>44624</v>
       </c>
-      <c r="N21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P21" s="10">
         <v>70.556773652403564</v>
       </c>
-      <c r="P21" s="10">
+      <c r="Q21" s="10">
         <v>10.712382845425132</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1638,10 +1708,10 @@
         <v>135</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G22" s="1">
         <v>13</v>
@@ -1653,25 +1723,28 @@
         <v>57</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K22" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="8">
+        <v>19</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="N22" s="8">
         <v>44624</v>
       </c>
-      <c r="N22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22" s="10">
+      <c r="O22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22" s="10">
         <v>67.72443542108627</v>
       </c>
-      <c r="P22" s="10">
+      <c r="Q22" s="10">
         <v>11.018343374790632</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1685,10 +1758,10 @@
         <v>135</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G23" s="1">
         <v>13</v>
@@ -1700,25 +1773,28 @@
         <v>45</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M23" s="8">
+        <v>66</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="8">
         <v>44624</v>
       </c>
-      <c r="N23" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="O23" s="10">
+      <c r="O23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" s="10">
         <v>64.892097189769061</v>
       </c>
-      <c r="P23" s="10">
+      <c r="Q23" s="10">
         <v>10.565689440934833</v>
       </c>
-      <c r="Q23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1732,10 +1808,10 @@
         <v>135</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G24" s="1">
         <v>13</v>
@@ -1747,22 +1823,25 @@
         <v>2</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M24" s="8">
+        <v>66</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="N24" s="8">
         <v>44624</v>
       </c>
-      <c r="N24" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="O24" s="10">
+      <c r="O24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P24" s="10">
         <v>71.438266673374784</v>
       </c>
-      <c r="P24" s="10">
+      <c r="Q24" s="10">
         <v>7.8288096371587814</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1776,10 +1855,10 @@
         <v>127</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G25" s="1">
         <v>14</v>
@@ -1791,22 +1870,25 @@
         <v>25</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M25" s="8">
+        <v>66</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="8">
         <v>44623</v>
       </c>
-      <c r="N25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O25" s="10">
+      <c r="O25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P25" s="10">
         <v>73.625152332785404</v>
       </c>
-      <c r="P25" s="10">
+      <c r="Q25" s="10">
         <v>8.21107174819217</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1820,10 +1902,10 @@
         <v>127</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G26" s="1">
         <v>14</v>
@@ -1835,22 +1917,25 @@
         <v>2</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M26" s="8">
+        <v>66</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="8">
         <v>44624</v>
       </c>
-      <c r="N26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="10">
+      <c r="O26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P26" s="10">
         <v>72.290858283822274</v>
       </c>
-      <c r="P26" s="10">
+      <c r="Q26" s="10">
         <v>8.3233759722974909</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1864,10 +1949,10 @@
         <v>55</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G27" s="1">
         <v>16</v>
@@ -1879,22 +1964,25 @@
         <v>27</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M27" s="8">
+        <v>66</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="8">
         <v>44623</v>
       </c>
-      <c r="N27" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="O27" s="10">
+      <c r="O27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="P27" s="10">
         <v>85.6024498414682</v>
       </c>
-      <c r="P27" s="10">
+      <c r="Q27" s="10">
         <v>6.5812358986766402</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -1908,10 +1996,10 @@
         <v>55</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G28" s="1">
         <v>16</v>
@@ -1923,22 +2011,25 @@
         <v>2</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M28" s="8">
+        <v>66</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="8">
         <v>44624</v>
       </c>
-      <c r="N28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O28" s="10">
+      <c r="O28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P28" s="10">
         <v>85.079732440535281</v>
       </c>
-      <c r="P28" s="10">
+      <c r="Q28" s="10">
         <v>6.7097485229042517</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1952,10 +2043,10 @@
         <v>47</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G29" s="1">
         <v>17</v>
@@ -1967,22 +2058,25 @@
         <v>27</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M29" s="8">
+        <v>66</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="8">
         <v>44623</v>
       </c>
-      <c r="N29" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O29" s="10">
+      <c r="O29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P29" s="10">
         <v>85.851976872899101</v>
       </c>
-      <c r="P29" s="10">
+      <c r="Q29" s="10">
         <v>4.3737367100923104</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1996,10 +2090,10 @@
         <v>47</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G30" s="1">
         <v>17</v>
@@ -2011,22 +2105,25 @@
         <v>15</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M30" s="8">
+        <v>66</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="8">
         <v>44623</v>
       </c>
-      <c r="N30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="O30" s="10">
+      <c r="O30" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P30" s="10">
         <v>88.141754337794396</v>
       </c>
-      <c r="P30" s="10">
+      <c r="Q30" s="10">
         <v>5.7023623899505402</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2040,10 +2137,10 @@
         <v>47</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G31" s="1">
         <v>17</v>
@@ -2055,22 +2152,25 @@
         <v>2</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M31" s="8">
+        <v>66</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="8">
         <v>44623</v>
       </c>
-      <c r="N31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O31" s="10">
+      <c r="O31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="P31" s="10">
         <v>87.026221726691602</v>
       </c>
-      <c r="P31" s="10">
+      <c r="Q31" s="10">
         <v>5.0504280501443297</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2084,10 +2184,10 @@
         <v>15</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G32" s="1">
         <v>23</v>
@@ -2099,22 +2199,25 @@
         <v>12</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M32" s="8">
+        <v>66</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1</v>
+      </c>
+      <c r="N32" s="8">
         <v>44623</v>
       </c>
-      <c r="N32" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="O32" s="10">
+      <c r="O32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="P32" s="10">
         <v>90.901229744206603</v>
       </c>
-      <c r="P32" s="10">
+      <c r="Q32" s="10">
         <v>5.97056322594677</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2128,10 +2231,10 @@
         <v>15</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G33" s="1">
         <v>23</v>
@@ -2143,22 +2246,25 @@
         <v>6</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M33" s="8">
+        <v>66</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="N33" s="8">
         <v>44623</v>
       </c>
-      <c r="N33" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O33" s="10">
+      <c r="O33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P33" s="10">
         <v>87.745446699639402</v>
       </c>
-      <c r="P33" s="10">
+      <c r="Q33" s="10">
         <v>4.9472738824534703</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2172,10 +2278,10 @@
         <v>15</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="G34" s="1">
         <v>23</v>
@@ -2187,22 +2293,25 @@
         <v>2</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M34" s="8">
+        <v>66</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1</v>
+      </c>
+      <c r="N34" s="8">
         <v>44623</v>
       </c>
-      <c r="N34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O34" s="10">
+      <c r="O34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="P34" s="10">
         <v>93.191007209101798</v>
       </c>
-      <c r="P34" s="10">
+      <c r="Q34" s="10">
         <v>5.2773672190642102</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2210,28 +2319,31 @@
         <v>20220221</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K35" t="s">
-        <v>74</v>
-      </c>
-      <c r="M35" s="8">
+        <v>72</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="N35" s="8">
         <v>44623</v>
       </c>
-      <c r="N35" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="O35" s="10">
+      <c r="O35" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P35" s="10">
         <v>4.6412027846145802</v>
       </c>
-      <c r="P35" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2239,24 +2351,27 @@
         <v>20220223</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K36" t="s">
-        <v>73</v>
-      </c>
-      <c r="M36" s="8">
+        <v>71</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1</v>
+      </c>
+      <c r="N36" s="8">
         <v>44623</v>
       </c>
-      <c r="N36" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="O36" s="10">
+      <c r="O36" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="P36" s="10">
         <v>3.7223561865220098</v>
       </c>
-      <c r="P36" s="10">
+      <c r="Q36" s="10">
         <v>0.26613775264241002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated DOC_ and btl data files
</commit_message>
<xml_diff>
--- a/data/input/DOC_20220226_AT46_wData20220307.xlsx
+++ b/data/input/DOC_20220226_AT46_wData20220307.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sosiknas1\Lab_data\LTER\DOC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4108801F-F51A-41D6-9E85-BF2DE32E9D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D916AAE4-3964-4E84-BB64-A4AC20195D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22365" yWindow="1920" windowWidth="21345" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="77">
   <si>
     <t>AT46</t>
   </si>
@@ -252,7 +263,10 @@
     <t>cast</t>
   </si>
   <si>
-    <t>quality_flag</t>
+    <t>quality_flag_C</t>
+  </si>
+  <si>
+    <t>quality_flag_N</t>
   </si>
 </sst>
 </file>
@@ -385,7 +399,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -668,22 +682,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="11" max="11" width="59.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="3" style="11" customWidth="1"/>
-    <col min="15" max="15" width="25.140625" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="3" style="11" customWidth="1"/>
+    <col min="16" max="16" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -720,23 +734,26 @@
       <c r="L1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,23 +787,30 @@
       <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="8">
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="8">
         <v>44623</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="10">
+      <c r="Q2" s="10">
         <v>90.7838052588273</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="R2" s="10">
         <v>6.1191052274216</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T2">
+        <f>Q2/R2</f>
+        <v>14.836124218292085</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,23 +844,30 @@
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="N3" s="8">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="8">
         <v>44623</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="10">
+      <c r="Q3" s="10">
         <v>85.851976872899101</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="R3" s="10">
         <v>5.0875635505130399</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <f t="shared" ref="T3:T36" si="0">Q3/R3</f>
+        <v>16.874870656749167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,20 +901,27 @@
       <c r="L4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="8">
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="8">
         <v>44623</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="10">
+      <c r="Q4" s="10">
         <v>80.993538790332906</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="R4" s="10">
         <v>7.3858384066653198</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>10.966058872509398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -917,20 +955,27 @@
       <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="N5" s="8">
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
         <v>44624</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="10">
+      <c r="Q5" s="10">
         <v>82.449704082883585</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="R5" s="10">
         <v>8.3443321729389623</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>9.8809230474155392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,20 +1012,27 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="N6" s="8">
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="8">
         <v>44624</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="10">
+      <c r="Q6" s="10">
         <v>81.14914060931946</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="R6" s="10">
         <v>7.6653512721553119</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>10.586486871658039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,20 +1066,27 @@
       <c r="L7" s="1">
         <v>1</v>
       </c>
-      <c r="N7" s="8">
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8">
         <v>44624</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="P7" s="10">
+      <c r="Q7" s="10">
         <v>76.033590946634263</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="R7" s="10">
         <v>9.1280940769299725</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>8.3296239396566829</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,20 +1120,27 @@
       <c r="L8" s="1">
         <v>1</v>
       </c>
-      <c r="N8" s="8">
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8">
         <v>44623</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="10">
+      <c r="Q8" s="10">
         <v>74.637938519181404</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="R8" s="10">
         <v>8.8712584214136498</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>8.4134555633075241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,20 +1174,27 @@
       <c r="L9" s="1">
         <v>1</v>
       </c>
-      <c r="N9" s="8">
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="8">
         <v>44623</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P9" s="10">
+      <c r="Q9" s="10">
         <v>74.006781910268003</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="R9" s="10">
         <v>8.1285484140394804</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>9.1045507931582037</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1155,20 +1228,27 @@
       <c r="L10" s="1">
         <v>1</v>
       </c>
-      <c r="N10" s="8">
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="8">
         <v>44623</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="10">
+      <c r="Q10" s="10">
         <v>70.850998865700802</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="R10" s="10">
         <v>8.7639780870151593</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>8.0843423114755044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1202,20 +1282,27 @@
       <c r="L11" s="1">
         <v>1</v>
       </c>
-      <c r="N11" s="8">
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="8">
         <v>44623</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="P11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="10">
+      <c r="Q11" s="10">
         <v>49.949440468195498</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="R11" s="10">
         <v>23.4696362330236</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>2.1282579743572145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,20 +1339,27 @@
       <c r="L12" s="1">
         <v>1</v>
       </c>
-      <c r="N12" s="8">
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8">
         <v>44624</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="P12" s="10">
+      <c r="Q12" s="10">
         <v>48.360490370244072</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="R12" s="10">
         <v>24.266853420328431</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>1.992862013570013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1299,20 +1393,27 @@
       <c r="L13" s="1">
         <v>1</v>
       </c>
-      <c r="N13" s="8">
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="8">
         <v>44623</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="P13" s="10">
+      <c r="Q13" s="10">
         <v>73.889357424888701</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="R13" s="10">
         <v>11.338706112578899</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>6.5165598871036572</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1346,20 +1447,27 @@
       <c r="L14" s="1">
         <v>1</v>
       </c>
-      <c r="N14" s="8">
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="8">
         <v>44624</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="P14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="P14" s="10">
+      <c r="Q14" s="10">
         <v>64.718688726627164</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="R14" s="10">
         <v>10.838120049273932</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>5.9713943407521857</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1393,20 +1501,27 @@
       <c r="L15" s="1">
         <v>1</v>
       </c>
-      <c r="N15" s="8">
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="8">
         <v>44623</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="P15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="P15" s="10">
+      <c r="Q15" s="10">
         <v>69.882246861322102</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="R15" s="10">
         <v>11.6522947823591</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>5.9972947961391929</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1443,20 +1558,27 @@
       <c r="L16" s="1">
         <v>1</v>
       </c>
-      <c r="N16" s="8">
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="O16" s="8">
         <v>44624</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="P16" s="10">
+      <c r="Q16" s="10">
         <v>71.95849206280036</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="R16" s="10">
         <v>9.1825801985977922</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>7.8364131329654647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1493,20 +1615,27 @@
       <c r="L17" s="1">
         <v>1</v>
       </c>
-      <c r="N17" s="8">
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="8">
         <v>44624</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="P17" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="P17" s="10">
+      <c r="Q17" s="10">
         <v>75.108745809877661</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="R17" s="10">
         <v>8.5580854194819622</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>8.7763491632015214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1540,20 +1669,27 @@
       <c r="L18" s="1">
         <v>1</v>
       </c>
-      <c r="N18" s="8">
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="O18" s="8">
         <v>44624</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="P18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="10">
+      <c r="Q18" s="10">
         <v>71.192604683923776</v>
       </c>
-      <c r="Q18" s="10">
+      <c r="R18" s="10">
         <v>8.6712489029459121</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <f t="shared" si="0"/>
+        <v>8.2101904213287291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1587,20 +1723,27 @@
       <c r="L19" s="1">
         <v>1</v>
       </c>
-      <c r="N19" s="8">
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="O19" s="8">
         <v>44624</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="P19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="P19" s="10">
+      <c r="Q19" s="10">
         <v>71.20705538918557</v>
       </c>
-      <c r="Q19" s="10">
+      <c r="R19" s="10">
         <v>8.0090329626754304</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <f t="shared" si="0"/>
+        <v>8.8908430919228909</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1634,20 +1777,27 @@
       <c r="L20" s="1">
         <v>1</v>
       </c>
-      <c r="N20" s="8">
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="8">
         <v>44624</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="P20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="P20" s="10">
+      <c r="Q20" s="10">
         <v>69.574125694599559</v>
       </c>
-      <c r="Q20" s="10">
+      <c r="R20" s="10">
         <v>8.331758452554082</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <f t="shared" si="0"/>
+        <v>8.350473203321414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,20 +1831,27 @@
       <c r="L21" s="1">
         <v>1</v>
       </c>
-      <c r="N21" s="8">
+      <c r="M21" s="1">
+        <v>1</v>
+      </c>
+      <c r="O21" s="8">
         <v>44624</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="P21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P21" s="10">
+      <c r="Q21" s="10">
         <v>70.556773652403564</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="R21" s="10">
         <v>10.712382845425132</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <f t="shared" si="0"/>
+        <v>6.5864686382578066</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,20 +1888,27 @@
       <c r="L22" s="1">
         <v>1</v>
       </c>
-      <c r="N22" s="8">
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="8">
         <v>44624</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="P22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P22" s="10">
+      <c r="Q22" s="10">
         <v>67.72443542108627</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="R22" s="10">
         <v>11.018343374790632</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>6.1465170504702256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1778,23 +1942,30 @@
       <c r="L23" s="1">
         <v>1</v>
       </c>
-      <c r="N23" s="8">
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="8">
         <v>44624</v>
       </c>
-      <c r="O23" s="9" t="s">
+      <c r="P23" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="10">
+      <c r="Q23" s="10">
         <v>64.892097189769061</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="R23" s="10">
         <v>10.565689440934833</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>6.141775939235588</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1828,20 +1999,27 @@
       <c r="L24" s="1">
         <v>1</v>
       </c>
-      <c r="N24" s="8">
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="8">
         <v>44624</v>
       </c>
-      <c r="O24" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="P24" s="10">
+      <c r="Q24" s="10">
         <v>71.438266673374784</v>
       </c>
-      <c r="Q24" s="10">
+      <c r="R24" s="10">
         <v>7.8288096371587814</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>9.1250483769970732</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1875,20 +2053,27 @@
       <c r="L25" s="1">
         <v>1</v>
       </c>
-      <c r="N25" s="8">
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="O25" s="8">
         <v>44623</v>
       </c>
-      <c r="O25" s="9" t="s">
+      <c r="P25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P25" s="10">
+      <c r="Q25" s="10">
         <v>73.625152332785404</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="R25" s="10">
         <v>8.21107174819217</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>8.9665703321853734</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1922,20 +2107,27 @@
       <c r="L26" s="1">
         <v>1</v>
       </c>
-      <c r="N26" s="8">
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="8">
         <v>44624</v>
       </c>
-      <c r="O26" s="9" t="s">
+      <c r="P26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="P26" s="10">
+      <c r="Q26" s="10">
         <v>72.290858283822274</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="R26" s="10">
         <v>8.3233759722974909</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>8.6852808913626323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1969,20 +2161,27 @@
       <c r="L27" s="1">
         <v>1</v>
       </c>
-      <c r="N27" s="8">
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="O27" s="8">
         <v>44623</v>
       </c>
-      <c r="O27" s="9" t="s">
+      <c r="P27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P27" s="10">
+      <c r="Q27" s="10">
         <v>85.6024498414682</v>
       </c>
-      <c r="Q27" s="10">
+      <c r="R27" s="10">
         <v>6.5812358986766402</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>13.007047788498388</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2016,20 +2215,27 @@
       <c r="L28" s="1">
         <v>1</v>
       </c>
-      <c r="N28" s="8">
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="O28" s="8">
         <v>44624</v>
       </c>
-      <c r="O28" s="9" t="s">
+      <c r="P28" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="P28" s="10">
+      <c r="Q28" s="10">
         <v>85.079732440535281</v>
       </c>
-      <c r="Q28" s="10">
+      <c r="R28" s="10">
         <v>6.7097485229042517</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>12.680018058815312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2063,20 +2269,27 @@
       <c r="L29" s="1">
         <v>1</v>
       </c>
-      <c r="N29" s="8">
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="O29" s="8">
         <v>44623</v>
       </c>
-      <c r="O29" s="9" t="s">
+      <c r="P29" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="P29" s="10">
+      <c r="Q29" s="10">
         <v>85.851976872899101</v>
       </c>
-      <c r="Q29" s="10">
+      <c r="R29" s="10">
         <v>4.3737367100923104</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>19.628976905445032</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2110,20 +2323,27 @@
       <c r="L30" s="1">
         <v>1</v>
       </c>
-      <c r="N30" s="8">
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="O30" s="8">
         <v>44623</v>
       </c>
-      <c r="O30" s="9" t="s">
+      <c r="P30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P30" s="10">
+      <c r="Q30" s="10">
         <v>88.141754337794396</v>
       </c>
-      <c r="Q30" s="10">
+      <c r="R30" s="10">
         <v>5.7023623899505402</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>15.457059427357597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2157,20 +2377,27 @@
       <c r="L31" s="1">
         <v>1</v>
       </c>
-      <c r="N31" s="8">
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="8">
         <v>44623</v>
       </c>
-      <c r="O31" s="9" t="s">
+      <c r="P31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="P31" s="10">
+      <c r="Q31" s="10">
         <v>87.026221726691602</v>
       </c>
-      <c r="Q31" s="10">
+      <c r="R31" s="10">
         <v>5.0504280501443297</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>17.231454613872696</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2204,20 +2431,27 @@
       <c r="L32" s="1">
         <v>1</v>
       </c>
-      <c r="N32" s="8">
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="8">
         <v>44623</v>
       </c>
-      <c r="O32" s="9" t="s">
+      <c r="P32" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="P32" s="10">
+      <c r="Q32" s="10">
         <v>90.901229744206603</v>
       </c>
-      <c r="Q32" s="10">
+      <c r="R32" s="10">
         <v>5.97056322594677</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>15.224900282299938</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2251,20 +2485,27 @@
       <c r="L33" s="1">
         <v>1</v>
       </c>
-      <c r="N33" s="8">
+      <c r="M33" s="1">
+        <v>1</v>
+      </c>
+      <c r="O33" s="8">
         <v>44623</v>
       </c>
-      <c r="O33" s="9" t="s">
+      <c r="P33" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="P33" s="10">
+      <c r="Q33" s="10">
         <v>87.745446699639402</v>
       </c>
-      <c r="Q33" s="10">
+      <c r="R33" s="10">
         <v>4.9472738824534703</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T33">
+        <f t="shared" si="0"/>
+        <v>17.73612069686434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2298,20 +2539,27 @@
       <c r="L34" s="1">
         <v>1</v>
       </c>
-      <c r="N34" s="8">
+      <c r="M34" s="1">
+        <v>1</v>
+      </c>
+      <c r="O34" s="8">
         <v>44623</v>
       </c>
-      <c r="O34" s="9" t="s">
+      <c r="P34" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P34" s="10">
+      <c r="Q34" s="10">
         <v>93.191007209101798</v>
       </c>
-      <c r="Q34" s="10">
+      <c r="R34" s="10">
         <v>5.2773672190642102</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <f t="shared" si="0"/>
+        <v>17.658617136297472</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2330,20 +2578,27 @@
       <c r="L35" s="1">
         <v>1</v>
       </c>
-      <c r="N35" s="8">
+      <c r="M35" s="1">
+        <v>1</v>
+      </c>
+      <c r="O35" s="8">
         <v>44623</v>
       </c>
-      <c r="O35" s="9" t="s">
+      <c r="P35" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="P35" s="10">
+      <c r="Q35" s="10">
         <v>4.6412027846145802</v>
       </c>
-      <c r="Q35" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="10">
+        <v>0</v>
+      </c>
+      <c r="T35" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2362,17 +2617,24 @@
       <c r="L36" s="1">
         <v>1</v>
       </c>
-      <c r="N36" s="8">
+      <c r="M36" s="1">
+        <v>1</v>
+      </c>
+      <c r="O36" s="8">
         <v>44623</v>
       </c>
-      <c r="O36" s="9" t="s">
+      <c r="P36" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="P36" s="10">
+      <c r="Q36" s="10">
         <v>3.7223561865220098</v>
       </c>
-      <c r="Q36" s="10">
+      <c r="R36" s="10">
         <v>0.26613775264241002</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="0"/>
+        <v>13.986577062306036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>